<commit_message>
two not used beacons added
</commit_message>
<xml_diff>
--- a/beacons_positions.xlsx
+++ b/beacons_positions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="78">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">AC233FA1046E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC233FA1046F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC233FA10542</t>
   </si>
 </sst>
 </file>
@@ -257,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -278,6 +284,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -332,6 +343,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,18 +371,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I75" activeCellId="0" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -724,7 +743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -744,7 +763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -764,7 +783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -784,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -804,7 +823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -824,7 +843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -844,7 +863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -864,7 +883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -884,7 +903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -904,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -924,7 +943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -944,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -964,7 +983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -984,7 +1003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +1023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1024,7 +1043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1044,7 +1063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1064,7 +1083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1084,7 +1103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
@@ -1104,7 +1123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -1124,7 +1143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1144,7 +1163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +1183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1184,7 +1203,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -1204,7 +1223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -1244,7 +1263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -1264,7 +1283,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -1284,7 +1303,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1324,7 +1343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -1344,7 +1363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -1364,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -1384,7 +1403,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
@@ -1404,7 +1423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -1424,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>60</v>
       </c>
@@ -1444,7 +1463,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -1464,7 +1483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -1484,7 +1503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -1504,7 +1523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -1524,7 +1543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -1544,7 +1563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -1564,7 +1583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
@@ -1584,7 +1603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -1604,7 +1623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>69</v>
       </c>
@@ -1624,7 +1643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -1644,7 +1663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -1664,7 +1683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -1684,7 +1703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -1704,7 +1723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -1724,7 +1743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -1741,6 +1760,40 @@
         <v>23</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="0" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>